<commit_message>
Skin gui torso conf file updated.
svn path=/trunk/iCub/; revision=14603
</commit_message>
<xml_diff>
--- a/app/skinGui/iniGenerators/torso_ini_generator.xlsx
+++ b/app/skinGui/iniGenerators/torso_ini_generator.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="13455" yWindow="-15" windowWidth="11685" windowHeight="12120" activeTab="5"/>
+    <workbookView xWindow="13455" yWindow="-15" windowWidth="11685" windowHeight="12120"/>
   </bookViews>
   <sheets>
     <sheet name="right upper" sheetId="4" r:id="rId1"/>
@@ -15516,8 +15516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15766,7 +15766,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="3">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="O7" s="42">
         <v>148</v>
@@ -15946,7 +15946,7 @@
       </c>
       <c r="C13" s="24">
         <f t="shared" ref="C13:C14" si="1">((+O13*COS($N$3)-P13*SIN($N$3))*$R$3)+$N$7</f>
-        <v>-33.602540378443777</v>
+        <v>-17.602540378443777</v>
       </c>
       <c r="D13" s="24">
         <f t="shared" ref="D13:D14" si="2">((O13*SIN($N$3)+P13*COS($N$3))*$R$4)+$N$9</f>
@@ -15994,7 +15994,7 @@
       </c>
       <c r="C14" s="24">
         <f t="shared" si="1"/>
-        <v>-49.602540378443749</v>
+        <v>-33.602540378443749</v>
       </c>
       <c r="D14" s="24">
         <f t="shared" si="2"/>
@@ -16042,7 +16042,7 @@
       </c>
       <c r="C15" s="24">
         <f t="shared" ref="C15:C23" si="6">((+O15*COS($N$3)-P15*SIN($N$3))*$R$3)+$N$7</f>
-        <v>-65.602540378443749</v>
+        <v>-49.602540378443749</v>
       </c>
       <c r="D15" s="24">
         <f t="shared" ref="D15:D23" si="7">((O15*SIN($N$3)+P15*COS($N$3))*$R$4)+$N$9</f>
@@ -16090,7 +16090,7 @@
       </c>
       <c r="C16" s="24">
         <f t="shared" si="6"/>
-        <v>-65.60254037844372</v>
+        <v>-49.60254037844372</v>
       </c>
       <c r="D16" s="24">
         <f t="shared" si="7"/>
@@ -16196,7 +16196,7 @@
       </c>
       <c r="C19" s="24">
         <f t="shared" si="6"/>
-        <v>-49.602540378443777</v>
+        <v>-33.602540378443777</v>
       </c>
       <c r="D19" s="24">
         <f t="shared" si="7"/>
@@ -16244,7 +16244,7 @@
       </c>
       <c r="C20" s="24">
         <f t="shared" si="6"/>
-        <v>-65.602540378443763</v>
+        <v>-49.602540378443763</v>
       </c>
       <c r="D20" s="24">
         <f t="shared" si="7"/>
@@ -16350,7 +16350,7 @@
       </c>
       <c r="C23" s="24">
         <f t="shared" si="6"/>
-        <v>-33.602540378443791</v>
+        <v>-17.602540378443791</v>
       </c>
       <c r="D23" s="24">
         <f t="shared" si="7"/>
@@ -18856,7 +18856,7 @@
   <dimension ref="A1:T30"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A4" sqref="A4:G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18981,7 +18981,7 @@
       </c>
       <c r="C4" s="24">
         <f t="shared" ref="C4:C5" si="1">((+O4*COS($N$3)-P4*SIN($N$3))*$R$3)+$N$7</f>
-        <v>30.397459621556152</v>
+        <v>47.397459621556152</v>
       </c>
       <c r="D4" s="24">
         <f t="shared" ref="D4:D5" si="2">((O4*SIN($N$3)+P4*COS($N$3))*$R$4)+$N$9</f>
@@ -19039,7 +19039,7 @@
       </c>
       <c r="C5" s="32">
         <f t="shared" si="1"/>
-        <v>30.397459621556152</v>
+        <v>47.397459621556152</v>
       </c>
       <c r="D5" s="32">
         <f t="shared" si="2"/>
@@ -19145,7 +19145,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="3">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="O7" s="42">
         <v>148</v>
@@ -19265,7 +19265,7 @@
       </c>
       <c r="C11" s="32">
         <f t="shared" ref="C11:C24" si="6">((+O11*COS($N$3)-P11*SIN($N$3))*$R$3)+$N$7</f>
-        <v>14.397459621556209</v>
+        <v>31.397459621556209</v>
       </c>
       <c r="D11" s="32">
         <f t="shared" ref="D11:D24" si="7">((O11*SIN($N$3)+P11*COS($N$3))*$R$4)+$N$9</f>
@@ -19315,7 +19315,7 @@
       </c>
       <c r="C12" s="24">
         <f t="shared" si="6"/>
-        <v>-1.6025403784437913</v>
+        <v>15.397459621556209</v>
       </c>
       <c r="D12" s="24">
         <f t="shared" si="7"/>
@@ -19363,7 +19363,7 @@
       </c>
       <c r="C13" s="32">
         <f t="shared" si="6"/>
-        <v>-17.602540378443791</v>
+        <v>-0.60254037844379127</v>
       </c>
       <c r="D13" s="32">
         <f t="shared" si="7"/>
@@ -19411,7 +19411,7 @@
       </c>
       <c r="C14" s="24">
         <f t="shared" si="6"/>
-        <v>-17.602540378443763</v>
+        <v>-0.60254037844376285</v>
       </c>
       <c r="D14" s="24">
         <f t="shared" si="7"/>
@@ -19575,7 +19575,7 @@
       </c>
       <c r="C19" s="32">
         <f t="shared" si="6"/>
-        <v>-1.6025403784437913</v>
+        <v>15.397459621556209</v>
       </c>
       <c r="D19" s="32">
         <f t="shared" si="7"/>
@@ -19710,7 +19710,7 @@
       </c>
       <c r="C23" s="32">
         <f t="shared" si="6"/>
-        <v>14.397459621556209</v>
+        <v>31.397459621556209</v>
       </c>
       <c r="D23" s="32">
         <f t="shared" si="7"/>
@@ -19758,7 +19758,7 @@
       </c>
       <c r="C24" s="24">
         <f t="shared" si="6"/>
-        <v>30.39745962155618</v>
+        <v>47.39745962155618</v>
       </c>
       <c r="D24" s="24">
         <f t="shared" si="7"/>
@@ -20678,8 +20678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView topLeftCell="A62" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -21443,7 +21443,7 @@
       </c>
       <c r="C27" s="63">
         <f>IF('left upper'!C4=0, "", 'left upper'!C4)</f>
-        <v>30.397459621556152</v>
+        <v>47.397459621556152</v>
       </c>
       <c r="D27" s="63">
         <f>IF('left upper'!D4=0, "", 'left upper'!D4)</f>
@@ -21473,7 +21473,7 @@
       </c>
       <c r="C28" s="63">
         <f>IF('left upper'!C5=0, "", 'left upper'!C5)</f>
-        <v>30.397459621556152</v>
+        <v>47.397459621556152</v>
       </c>
       <c r="D28" s="63">
         <f>IF('left upper'!D5=0, "", 'left upper'!D5)</f>
@@ -21653,7 +21653,7 @@
       </c>
       <c r="C34" s="63">
         <f>IF('left upper'!C11=0, "", 'left upper'!C11)</f>
-        <v>14.397459621556209</v>
+        <v>31.397459621556209</v>
       </c>
       <c r="D34" s="63">
         <f>IF('left upper'!D11=0, "", 'left upper'!D11)</f>
@@ -21683,7 +21683,7 @@
       </c>
       <c r="C35" s="63">
         <f>IF('left upper'!C12=0, "", 'left upper'!C12)</f>
-        <v>-1.6025403784437913</v>
+        <v>15.397459621556209</v>
       </c>
       <c r="D35" s="63">
         <f>IF('left upper'!D12=0, "", 'left upper'!D12)</f>
@@ -21713,7 +21713,7 @@
       </c>
       <c r="C36" s="63">
         <f>IF('left upper'!C13=0, "", 'left upper'!C13)</f>
-        <v>-17.602540378443791</v>
+        <v>-0.60254037844379127</v>
       </c>
       <c r="D36" s="63">
         <f>IF('left upper'!D13=0, "", 'left upper'!D13)</f>
@@ -21743,7 +21743,7 @@
       </c>
       <c r="C37" s="63">
         <f>IF('left upper'!C14=0, "", 'left upper'!C14)</f>
-        <v>-17.602540378443763</v>
+        <v>-0.60254037844376285</v>
       </c>
       <c r="D37" s="63">
         <f>IF('left upper'!D14=0, "", 'left upper'!D14)</f>
@@ -21893,7 +21893,7 @@
       </c>
       <c r="C42" s="63">
         <f>IF('left upper'!C19=0, "", 'left upper'!C19)</f>
-        <v>-1.6025403784437913</v>
+        <v>15.397459621556209</v>
       </c>
       <c r="D42" s="63">
         <f>IF('left upper'!D19=0, "", 'left upper'!D19)</f>
@@ -22013,7 +22013,7 @@
       </c>
       <c r="C46" s="63">
         <f>IF('left upper'!C23=0, "", 'left upper'!C23)</f>
-        <v>14.397459621556209</v>
+        <v>31.397459621556209</v>
       </c>
       <c r="D46" s="63">
         <f>IF('left upper'!D23=0, "", 'left upper'!D23)</f>
@@ -22043,7 +22043,7 @@
       </c>
       <c r="C47" s="63">
         <f>IF('left upper'!C24=0, "", 'left upper'!C24)</f>
-        <v>30.39745962155618</v>
+        <v>47.39745962155618</v>
       </c>
       <c r="D47" s="63">
         <f>IF('left upper'!D24=0, "", 'left upper'!D24)</f>
@@ -23093,7 +23093,7 @@
       </c>
       <c r="C82" s="65">
         <f>IF('right upper'!C13=0, "", 'right upper'!C13)</f>
-        <v>-33.602540378443777</v>
+        <v>-17.602540378443777</v>
       </c>
       <c r="D82" s="65">
         <f>IF('right upper'!D13=0, "", 'right upper'!D13)</f>
@@ -23123,7 +23123,7 @@
       </c>
       <c r="C83" s="65">
         <f>IF('right upper'!C14=0, "", 'right upper'!C14)</f>
-        <v>-49.602540378443749</v>
+        <v>-33.602540378443749</v>
       </c>
       <c r="D83" s="65">
         <f>IF('right upper'!D14=0, "", 'right upper'!D14)</f>
@@ -23153,7 +23153,7 @@
       </c>
       <c r="C84" s="65">
         <f>IF('right upper'!C15=0, "", 'right upper'!C15)</f>
-        <v>-65.602540378443749</v>
+        <v>-49.602540378443749</v>
       </c>
       <c r="D84" s="65">
         <f>IF('right upper'!D15=0, "", 'right upper'!D15)</f>
@@ -23183,7 +23183,7 @@
       </c>
       <c r="C85" s="65">
         <f>IF('right upper'!C16=0, "", 'right upper'!C16)</f>
-        <v>-65.60254037844372</v>
+        <v>-49.60254037844372</v>
       </c>
       <c r="D85" s="65">
         <f>IF('right upper'!D16=0, "", 'right upper'!D16)</f>
@@ -23273,7 +23273,7 @@
       </c>
       <c r="C88" s="65">
         <f>IF('right upper'!C19=0, "", 'right upper'!C19)</f>
-        <v>-49.602540378443777</v>
+        <v>-33.602540378443777</v>
       </c>
       <c r="D88" s="65">
         <f>IF('right upper'!D19=0, "", 'right upper'!D19)</f>
@@ -23303,7 +23303,7 @@
       </c>
       <c r="C89" s="65">
         <f>IF('right upper'!C20=0, "", 'right upper'!C20)</f>
-        <v>-65.602540378443763</v>
+        <v>-49.602540378443763</v>
       </c>
       <c r="D89" s="65">
         <f>IF('right upper'!D20=0, "", 'right upper'!D20)</f>
@@ -23393,7 +23393,7 @@
       </c>
       <c r="C92" s="65">
         <f>IF('right upper'!C23=0, "", 'right upper'!C23)</f>
-        <v>-33.602540378443791</v>
+        <v>-17.602540378443791</v>
       </c>
       <c r="D92" s="65">
         <f>IF('right upper'!D23=0, "", 'right upper'!D23)</f>

</xml_diff>